<commit_message>
Still fleshing these out. Physical connections provisionally complete for InterfaceControlDocument
</commit_message>
<xml_diff>
--- a/doc/systems/InterfaceControlDocument.xlsx
+++ b/doc/systems/InterfaceControlDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
   </bookViews>
   <sheets>
     <sheet name="Control Box Physical Interface" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="73">
   <si>
     <t>Interface</t>
   </si>
@@ -94,9 +94,6 @@
     <t>SMA</t>
   </si>
   <si>
-    <t>GPS external antenna</t>
-  </si>
-  <si>
     <t>Primary Relay</t>
   </si>
   <si>
@@ -127,15 +124,9 @@
     <t>White</t>
   </si>
   <si>
-    <t>Optional for next build</t>
-  </si>
-  <si>
     <t>0 or 12V</t>
   </si>
   <si>
-    <t>PWM</t>
-  </si>
-  <si>
     <t>Battery Monitor</t>
   </si>
   <si>
@@ -206,6 +197,54 @@
   </si>
   <si>
     <t>Yellow</t>
+  </si>
+  <si>
+    <t>Boatse 0.3</t>
+  </si>
+  <si>
+    <t>Boatse 0.2</t>
+  </si>
+  <si>
+    <t>Encoding</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>Ethernet</t>
+  </si>
+  <si>
+    <t>PCM</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>digital</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relay </t>
+  </si>
+  <si>
+    <t>ground</t>
+  </si>
+  <si>
+    <t>analog</t>
+  </si>
+  <si>
+    <t>motor</t>
+  </si>
+  <si>
+    <t>relay</t>
+  </si>
+  <si>
+    <t>ext ant</t>
+  </si>
+  <si>
+    <t>network</t>
   </si>
 </sst>
 </file>
@@ -545,21 +584,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F39"/>
+  <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -576,10 +616,16 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -590,13 +636,19 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -612,8 +664,14 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>11</v>
@@ -627,13 +685,19 @@
       <c r="E5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -644,8 +708,14 @@
       <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" t="str">
         <f>B6</f>
@@ -661,10 +731,13 @@
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" t="str">
         <f>B7</f>
@@ -679,8 +752,14 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
@@ -691,30 +770,42 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
       <c r="B11" t="str">
         <f>B10</f>
@@ -724,13 +815,19 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
       <c r="B12" t="str">
         <f>B11</f>
@@ -745,25 +842,37 @@
       <c r="E12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
       <c r="B14" t="str">
         <f>B13</f>
@@ -773,13 +882,19 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
       <c r="B15" t="str">
         <f>B14</f>
@@ -794,53 +909,71 @@
       <c r="E15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>23</v>
-      </c>
-      <c r="B20" t="s">
-        <v>24</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -851,58 +984,82 @@
       <c r="E20" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" t="s">
         <v>32</v>
       </c>
-      <c r="E23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -914,69 +1071,81 @@
         <v>13</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25">
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+      <c r="G26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B28" t="s">
         <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>39</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -988,69 +1157,81 @@
         <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C29">
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
       </c>
       <c r="F30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G31" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1062,69 +1243,81 @@
         <v>13</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G32" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
         <v>18</v>
       </c>
       <c r="F33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E34" t="s">
         <v>18</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="G35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1136,61 +1329,73 @@
         <v>13</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G36" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C37">
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E37" t="s">
         <v>18</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C38">
         <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>18</v>
       </c>
       <c r="F38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C39">
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F39" t="s">
-        <v>33</v>
+        <v>63</v>
+      </c>
+      <c r="G39" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1214,20 +1419,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F16"/>
+  <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1244,10 +1452,16 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1263,8 +1477,14 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>11</v>
@@ -1278,75 +1498,105 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1357,58 +1607,82 @@
       <c r="E9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
       <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1420,61 +1694,73 @@
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="G13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>70</v>
+      </c>
+      <c r="G16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1490,21 +1776,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F5"/>
+  <dimension ref="A2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.21875" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1521,10 +1809,16 @@
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1540,8 +1834,14 @@
       <c r="E3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1557,8 +1857,14 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>11</v>
@@ -1571,6 +1877,12 @@
       </c>
       <c r="E5" t="s">
         <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mounting plates Updated ICD
</commit_message>
<xml_diff>
--- a/doc/systems/InterfaceControlDocument.xlsx
+++ b/doc/systems/InterfaceControlDocument.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6264"/>
   </bookViews>
   <sheets>
     <sheet name="Control Box Physical Interface" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="81">
   <si>
     <t>Interface</t>
   </si>
@@ -263,6 +263,15 @@
   </si>
   <si>
     <t>8-14V</t>
+  </si>
+  <si>
+    <t>Air Horn</t>
+  </si>
+  <si>
+    <t>M12A-2 female</t>
+  </si>
+  <si>
+    <t>Horn</t>
   </si>
 </sst>
 </file>
@@ -310,9 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -321,6 +327,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -340,98 +349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D01D6C5D-28BB-4289-B600-292454AA1F3A}" diskRevisions="1" revisionId="5" version="2">
-  <header guid="{825602CF-4ADE-4F82-8F15-0BCB98C78B43}" dateTime="2014-08-05T21:09:34" maxSheetId="4" userName="Pierce" r:id="rId1">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D01D6C5D-28BB-4289-B600-292454AA1F3A}" dateTime="2014-08-05T21:34:09" maxSheetId="4" userName="Pierce" r:id="rId2" minRId="1" maxRId="5">
-    <sheetIdMap count="3">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="1" sId="1">
-    <oc r="E4" t="inlineStr">
-      <is>
-        <t>12V</t>
-      </is>
-    </oc>
-    <nc r="E4" t="inlineStr">
-      <is>
-        <t>8V-14V</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="2" sId="1">
-    <oc r="E10" t="inlineStr">
-      <is>
-        <t>12V</t>
-      </is>
-    </oc>
-    <nc r="E10" t="inlineStr">
-      <is>
-        <t>5V</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="3" sId="1">
-    <oc r="E13" t="inlineStr">
-      <is>
-        <t>12V</t>
-      </is>
-    </oc>
-    <nc r="E13" t="inlineStr">
-      <is>
-        <t>5V</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="4" sId="2">
-    <oc r="E3" t="inlineStr">
-      <is>
-        <t>12V</t>
-      </is>
-    </oc>
-    <nc r="E3" t="inlineStr">
-      <is>
-        <t>8-14V</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="5" sId="3">
-    <oc r="E4" t="inlineStr">
-      <is>
-        <t>12V</t>
-      </is>
-    </oc>
-    <nc r="E4" t="inlineStr">
-      <is>
-        <t>8-14V</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -697,15 +614,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H41"/>
+  <dimension ref="A2:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -713,7 +630,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -739,7 +656,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -762,7 +679,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -785,7 +702,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -806,7 +723,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
@@ -829,7 +746,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="6"/>
       <c r="B7" t="str">
         <f>B6</f>
         <v>M12A-3 female</v>
@@ -851,7 +768,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="6"/>
       <c r="B8" t="str">
         <f>B7</f>
         <v>M12A-3 female</v>
@@ -873,7 +790,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B9" t="s">
@@ -896,7 +813,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B10" t="s">
@@ -919,7 +836,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" t="str">
         <f>B10</f>
         <v>M12A-3 female</v>
@@ -941,7 +858,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" t="str">
         <f>B11</f>
         <v>M12A-3 female</v>
@@ -963,7 +880,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B13" t="s">
@@ -986,7 +903,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
+      <c r="A14" s="7"/>
       <c r="B14" t="str">
         <f>B13</f>
         <v>M12A-3 female</v>
@@ -1008,7 +925,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
+      <c r="A15" s="7"/>
       <c r="B15" t="str">
         <f>B14</f>
         <v>M12A-3 female</v>
@@ -1030,7 +947,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B16" t="s">
@@ -1053,7 +970,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
+      <c r="A17" s="7"/>
       <c r="B17" t="str">
         <f>B16</f>
         <v>M8A-3 female</v>
@@ -1075,7 +992,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
+      <c r="A18" s="7"/>
       <c r="B18" t="str">
         <f>B17</f>
         <v>M8A-3 female</v>
@@ -1097,7 +1014,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B19" t="str">
@@ -1121,7 +1038,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
+      <c r="A20" s="7"/>
       <c r="B20" t="str">
         <f>B19</f>
         <v>M8A-3 female</v>
@@ -1143,7 +1060,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
+      <c r="A21" s="7"/>
       <c r="B21" t="str">
         <f>B20</f>
         <v>M8A-3 female</v>
@@ -1165,7 +1082,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
@@ -1188,7 +1105,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="A23" s="6"/>
       <c r="B23" t="s">
         <v>23</v>
       </c>
@@ -1209,7 +1126,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+      <c r="A24" s="6"/>
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1230,7 +1147,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
+      <c r="A25" s="6"/>
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -1251,7 +1168,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1274,7 +1191,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
+      <c r="A27" s="6"/>
       <c r="B27" t="s">
         <v>23</v>
       </c>
@@ -1295,7 +1212,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="6"/>
       <c r="B28" t="s">
         <v>23</v>
       </c>
@@ -1316,7 +1233,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="6"/>
       <c r="B29" t="s">
         <v>23</v>
       </c>
@@ -1337,7 +1254,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B30" t="s">
@@ -1360,7 +1277,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="6"/>
       <c r="B31" t="s">
         <v>36</v>
       </c>
@@ -1381,7 +1298,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
+      <c r="A32" s="6"/>
       <c r="B32" t="s">
         <v>36</v>
       </c>
@@ -1402,7 +1319,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="6"/>
       <c r="B33" t="s">
         <v>36</v>
       </c>
@@ -1423,7 +1340,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
@@ -1446,7 +1363,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="6"/>
       <c r="B35" t="s">
         <v>36</v>
       </c>
@@ -1467,7 +1384,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
+      <c r="A36" s="6"/>
       <c r="B36" t="s">
         <v>36</v>
       </c>
@@ -1488,7 +1405,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="3"/>
+      <c r="A37" s="6"/>
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -1509,7 +1426,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
@@ -1532,7 +1449,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="3"/>
+      <c r="A39" s="6"/>
       <c r="B39" t="s">
         <v>36</v>
       </c>
@@ -1553,7 +1470,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="3"/>
+      <c r="A40" s="6"/>
       <c r="B40" t="s">
         <v>36</v>
       </c>
@@ -1574,7 +1491,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="3"/>
+      <c r="A41" s="6"/>
       <c r="B41" t="s">
         <v>36</v>
       </c>
@@ -1592,6 +1509,50 @@
       </c>
       <c r="G41" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="6"/>
+      <c r="B43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1602,17 +1563,18 @@
       <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A30:A33"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1625,7 +1587,7 @@
   <dimension ref="A2:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1639,7 +1601,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1665,7 +1627,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
@@ -1688,7 +1650,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1709,7 +1671,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B5" t="s">
@@ -1732,7 +1694,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>49</v>
       </c>
@@ -1753,7 +1715,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="6"/>
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -1774,7 +1736,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="6"/>
       <c r="B8" t="s">
         <v>49</v>
       </c>
@@ -1795,7 +1757,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B9" t="s">
@@ -1818,7 +1780,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="6"/>
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1839,7 +1801,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="6"/>
       <c r="B11" t="s">
         <v>23</v>
       </c>
@@ -1860,7 +1822,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="6"/>
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -1881,7 +1843,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B13" t="s">
@@ -1904,7 +1866,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="6"/>
       <c r="B14" t="s">
         <v>23</v>
       </c>
@@ -1925,7 +1887,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="6"/>
       <c r="B15" t="s">
         <v>23</v>
       </c>
@@ -1946,7 +1908,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="3"/>
+      <c r="A16" s="6"/>
       <c r="B16" t="s">
         <v>23</v>
       </c>
@@ -1987,13 +1949,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
@@ -2002,7 +1964,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -2028,7 +1990,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
@@ -2051,7 +2013,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
@@ -2074,7 +2036,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -2095,7 +2057,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B6" t="s">

</xml_diff>

<commit_message>
Not sure when I made these changes...
</commit_message>
<xml_diff>
--- a/doc/systems/InterfaceControlDocument.xlsx
+++ b/doc/systems/InterfaceControlDocument.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="89">
   <si>
     <t>Interface</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>network - white/green</t>
+  </si>
+  <si>
+    <t>Arduino Pin</t>
   </si>
 </sst>
 </file>
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H46"/>
+  <dimension ref="A2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,10 +653,11 @@
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -676,10 +680,13 @@
         <v>57</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -702,7 +709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="C4" t="s">
         <v>81</v>
@@ -711,7 +718,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="C5" t="s">
         <v>82</v>
@@ -720,7 +727,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="C6" t="s">
         <v>83</v>
@@ -729,7 +736,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -752,7 +759,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" t="s">
         <v>11</v>
@@ -773,15 +780,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>24</v>
       </c>
-      <c r="C9">
-        <v>1</v>
+      <c r="C9" t="s">
+        <v>81</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -796,14 +803,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" t="str">
         <f>B9</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C10">
-        <v>2</v>
+      <c r="C10" t="s">
+        <v>83</v>
       </c>
       <c r="D10" t="s">
         <v>17</v>
@@ -818,14 +825,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" t="str">
         <f>B10</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C11">
-        <v>3</v>
+      <c r="C11" t="s">
+        <v>80</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -840,7 +847,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
@@ -863,15 +870,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>45</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="C13">
-        <v>1</v>
+      <c r="C13" t="s">
+        <v>81</v>
       </c>
       <c r="D13" t="s">
         <v>39</v>
@@ -886,14 +893,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" t="str">
         <f>B13</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C14">
-        <v>2</v>
+      <c r="C14" t="s">
+        <v>80</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
@@ -907,15 +914,18 @@
       <c r="G14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" t="str">
         <f>B14</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C15">
-        <v>3</v>
+      <c r="C15" t="s">
+        <v>83</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
@@ -930,15 +940,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
         <v>48</v>
       </c>
       <c r="B16" t="s">
         <v>24</v>
       </c>
-      <c r="C16">
-        <v>1</v>
+      <c r="C16" t="s">
+        <v>81</v>
       </c>
       <c r="D16" t="s">
         <v>39</v>
@@ -953,14 +963,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" t="str">
         <f>B16</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C17">
-        <v>2</v>
+      <c r="C17" t="s">
+        <v>80</v>
       </c>
       <c r="D17" t="s">
         <v>46</v>
@@ -974,15 +984,18 @@
       <c r="G17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" t="str">
         <f>B17</f>
         <v>M12A-3 female</v>
       </c>
-      <c r="C18">
-        <v>3</v>
+      <c r="C18" t="s">
+        <v>83</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
@@ -997,15 +1010,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>73</v>
       </c>
-      <c r="C19">
-        <v>1</v>
+      <c r="C19" t="s">
+        <v>81</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>74</v>
@@ -1020,14 +1033,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" t="str">
         <f>B19</f>
         <v>M8A-3 female</v>
       </c>
-      <c r="C20">
-        <v>2</v>
+      <c r="C20" t="s">
+        <v>80</v>
       </c>
       <c r="D20" t="s">
         <v>46</v>
@@ -1042,14 +1055,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" t="str">
         <f>B20</f>
         <v>M8A-3 female</v>
       </c>
-      <c r="C21">
-        <v>3</v>
+      <c r="C21" t="s">
+        <v>83</v>
       </c>
       <c r="D21" t="s">
         <v>13</v>
@@ -1064,7 +1077,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
         <v>72</v>
       </c>
@@ -1072,8 +1085,8 @@
         <f>B21</f>
         <v>M8A-3 female</v>
       </c>
-      <c r="C22">
-        <v>1</v>
+      <c r="C22" t="s">
+        <v>81</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>74</v>
@@ -1088,14 +1101,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" t="str">
         <f>B22</f>
         <v>M8A-3 female</v>
       </c>
-      <c r="C23">
-        <v>2</v>
+      <c r="C23" t="s">
+        <v>80</v>
       </c>
       <c r="D23" t="s">
         <v>46</v>
@@ -1110,14 +1123,14 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" t="str">
         <f>B23</f>
         <v>M8A-3 female</v>
       </c>
-      <c r="C24">
-        <v>3</v>
+      <c r="C24" t="s">
+        <v>83</v>
       </c>
       <c r="D24" t="s">
         <v>13</v>
@@ -1132,7 +1145,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1168,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" t="s">
         <v>23</v>
@@ -1176,7 +1189,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" t="s">
         <v>23</v>
@@ -1197,7 +1210,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" t="s">
         <v>23</v>
@@ -1218,7 +1231,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -1241,7 +1254,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" t="s">
         <v>23</v>
@@ -1262,7 +1275,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" t="s">
         <v>23</v>
@@ -1283,7 +1296,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" t="s">
         <v>23</v>
@@ -1569,8 +1582,8 @@
       <c r="B45" t="s">
         <v>78</v>
       </c>
-      <c r="C45">
-        <v>1</v>
+      <c r="C45" t="s">
+        <v>81</v>
       </c>
       <c r="D45" t="s">
         <v>79</v>
@@ -1590,8 +1603,8 @@
       <c r="B46" t="s">
         <v>78</v>
       </c>
-      <c r="C46">
-        <v>1</v>
+      <c r="C46" t="s">
+        <v>83</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
some updates to the ICD
</commit_message>
<xml_diff>
--- a/doc/systems/InterfaceControlDocument.xlsx
+++ b/doc/systems/InterfaceControlDocument.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="89">
   <si>
     <t>Interface</t>
   </si>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1410,8 +1410,8 @@
       <c r="B37" t="s">
         <v>36</v>
       </c>
-      <c r="C37">
-        <v>1</v>
+      <c r="C37" t="s">
+        <v>80</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -1431,8 +1431,8 @@
       <c r="B38" t="s">
         <v>36</v>
       </c>
-      <c r="C38">
-        <v>2</v>
+      <c r="C38" t="s">
+        <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>41</v>
@@ -1452,8 +1452,8 @@
       <c r="B39" t="s">
         <v>36</v>
       </c>
-      <c r="C39">
-        <v>3</v>
+      <c r="C39" t="s">
+        <v>81</v>
       </c>
       <c r="D39" t="s">
         <v>42</v>
@@ -1473,8 +1473,8 @@
       <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="C40">
-        <v>4</v>
+      <c r="C40" t="s">
+        <v>83</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>

</xml_diff>